<commit_message>
feat(app): Implementar paginación en todas las tablas de gestión
Se añade paginación a todas las vistas de tabla principales del panel de administración para mejorar el rendimiento y la usabilidad con grandes volúmenes de datos.

- Los módulos actualizados incluyen: Gestión de Libros, Usuarios, Recursos, Préstamos, Reservas, Sanciones e Inventario.
- La página de Reportes también fue actualizada para soportar paginación en sus resultados.
- El backend ahora acepta parámetros 'page' y 'limit' en los endpoints de listado, devolviendo los datos en un formato paginado.
- El frontend se ha actualizado con controles de paginación y la lógica necesaria para solicitar y renderizar los datos página por página.
</commit_message>
<xml_diff>
--- a/frontend/public/templates/plantilla_libros.xlsx
+++ b/frontend/public/templates/plantilla_libros.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyect_Sophia\frontend\public\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DDDBCA-2FBC-4C38-870B-CD1D6CDDAA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="plantilla_libros.xlsx&#10;Obligator" sheetId="1" r:id="rId4"/>
+    <sheet name="y las plantillas debo modificar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>titulo</t>
   </si>
@@ -22,45 +31,69 @@
     <t>editorial</t>
   </si>
   <si>
+    <t>sede</t>
+  </si>
+  <si>
+    <t>cantidadEjemplares</t>
+  </si>
+  <si>
+    <t>añoPublicacion</t>
+  </si>
+  <si>
     <t>lugarPublicacion</t>
   </si>
   <si>
-    <t>añoPublicacion</t>
-  </si>
-  <si>
-    <t>sede</t>
-  </si>
-  <si>
-    <t>cantidadEjemplares</t>
+    <t>edicion</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>numeroPaginas</t>
+  </si>
+  <si>
+    <t>idioma</t>
+  </si>
+  <si>
+    <t>descriptores</t>
   </si>
   <si>
     <t>tipoDocumento</t>
   </si>
   <si>
-    <t>isbn</t>
-  </si>
-  <si>
-    <t>pais</t>
-  </si>
-  <si>
-    <t>numeroPaginas</t>
-  </si>
-  <si>
-    <t>descriptores</t>
-  </si>
-  <si>
-    <t>idioma</t>
-  </si>
-  <si>
     <t>cdd</t>
   </si>
   <si>
-    <t>edicion</t>
-  </si>
-  <si>
     <t>ubicacionEstanteria</t>
   </si>
   <si>
+    <t>(Ej: Madrid)</t>
+  </si>
+  <si>
+    <t>(Ej: 1ra)</t>
+  </si>
+  <si>
+    <t>(Ej: ...)</t>
+  </si>
+  <si>
+    <t>(Ej: 496)</t>
+  </si>
+  <si>
+    <t>(Ej: Español)</t>
+  </si>
+  <si>
+    <t>(Ej: historia,...)</t>
+  </si>
+  <si>
+    <t>(Ej: Ensayo)</t>
+  </si>
+  <si>
+    <t>(Ej: 909)</t>
+  </si>
+  <si>
+    <t>(Ej: Pasillo 1)</t>
+  </si>
+  <si>
     <t>Cien años de soledad</t>
   </si>
   <si>
@@ -70,45 +103,172 @@
     <t>Sudamericana</t>
   </si>
   <si>
-    <t>Buenos Aires</t>
-  </si>
-  <si>
     <t>Media</t>
   </si>
   <si>
-    <t>Novela</t>
-  </si>
-  <si>
-    <t>978-0307474728</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>realismo magico, clasico</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
-    <t>1ra</t>
-  </si>
-  <si>
-    <t>Pasillo A, Estante 3</t>
+    <t>El Hobbit</t>
+  </si>
+  <si>
+    <t>J.R.R. Tolkien</t>
+  </si>
+  <si>
+    <t>Minotauro</t>
+  </si>
+  <si>
+    <t>Basica</t>
+  </si>
+  <si>
+    <t>George Orwell</t>
+  </si>
+  <si>
+    <t>Debolsillo</t>
+  </si>
+  <si>
+    <t>Un mundo feliz</t>
+  </si>
+  <si>
+    <t>Aldous Huxley</t>
+  </si>
+  <si>
+    <t>Cátedra</t>
+  </si>
+  <si>
+    <t>Orgullo y prejuicio</t>
+  </si>
+  <si>
+    <t>Jane Austen</t>
+  </si>
+  <si>
+    <t>Alianza Editorial</t>
+  </si>
+  <si>
+    <t>Crónica de una muerte anunciada</t>
+  </si>
+  <si>
+    <t>La Oveja Negra</t>
+  </si>
+  <si>
+    <t>El señor de los anillos</t>
+  </si>
+  <si>
+    <t>Don Quijote de la Mancha</t>
+  </si>
+  <si>
+    <t>Miguel de Cervantes</t>
+  </si>
+  <si>
+    <t>Real Academia Española</t>
+  </si>
+  <si>
+    <t>La Odisea</t>
+  </si>
+  <si>
+    <t>Homero</t>
+  </si>
+  <si>
+    <t>Gredos</t>
+  </si>
+  <si>
+    <t>El principito</t>
+  </si>
+  <si>
+    <t>Antoine de Saint-Exupéry</t>
+  </si>
+  <si>
+    <t>Salamandra</t>
+  </si>
+  <si>
+    <t>Harry Potter y la piedra filosofal</t>
+  </si>
+  <si>
+    <t>J.K. Rowling</t>
+  </si>
+  <si>
+    <t>Matilda</t>
+  </si>
+  <si>
+    <t>Roald Dahl</t>
+  </si>
+  <si>
+    <t>Alfaguara</t>
+  </si>
+  <si>
+    <t>Papelucho</t>
+  </si>
+  <si>
+    <t>Marcela Paz</t>
+  </si>
+  <si>
+    <t>Universitaria</t>
+  </si>
+  <si>
+    <t>El alquimista</t>
+  </si>
+  <si>
+    <t>Paulo Coelho</t>
+  </si>
+  <si>
+    <t>Planeta</t>
+  </si>
+  <si>
+    <t>Rayuela</t>
+  </si>
+  <si>
+    <t>Julio Cortázar</t>
+  </si>
+  <si>
+    <t>El túnel</t>
+  </si>
+  <si>
+    <t>Ernesto Sabato</t>
+  </si>
+  <si>
+    <t>La casa de los espíritus</t>
+  </si>
+  <si>
+    <t>Isabel Allende</t>
+  </si>
+  <si>
+    <t>Plaza &amp; Janés</t>
+  </si>
+  <si>
+    <t>Veinte poemas de amor y una canción desesperada</t>
+  </si>
+  <si>
+    <t>Pablo Neruda</t>
+  </si>
+  <si>
+    <t>Nascimento</t>
+  </si>
+  <si>
+    <t>Fahrenheit 451</t>
+  </si>
+  <si>
+    <t>Ray Bradbury</t>
+  </si>
+  <si>
+    <t>Moby Dick</t>
+  </si>
+  <si>
+    <t>Herman Melville</t>
+  </si>
+  <si>
+    <t>Alba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -119,36 +279,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -338,20 +505,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -397,61 +572,435 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1967</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1">
-        <v>1967.0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1">
-        <v>496.0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1984</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="1">
-        <v>863.44</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>-800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>1851</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(app): Implementar paginación y modales de confirmación
Se introduce un sistema de paginación completo en todas las vistas de tabla principales del panel de administración (Libros, Usuarios, Recursos, Préstamos, etc.) para mejorar el rendimiento y la escalabilidad.

- El backend ahora sirve los datos en formato paginado en todos los endpoints de listado.
- El frontend se ha actualizado con controles de paginación y la lógica de estado necesaria.

Además, se realizan las siguientes mejoras de usabilidad:
- Se reemplazan todas las alertas nativas ('window.confirm') por modales personalizados y consistentes para las operaciones de eliminación.
- Se mejora el componente de importación masiva para que se resetee correctamente después de un intento de subida y muestre notificaciones de éxito.
- Se corrigen y refinan lógicas de negocio en el módulo de préstamos (ordenamiento del historial, cálculo de vencimiento y estado final).
</commit_message>
<xml_diff>
--- a/frontend/public/templates/plantilla_libros.xlsx
+++ b/frontend/public/templates/plantilla_libros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyect_Sophia\frontend\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DDDBCA-2FBC-4C38-870B-CD1D6CDDAA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BE8A45-0653-4867-9E9A-F933300FFCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>titulo</t>
   </si>
@@ -67,33 +67,6 @@
     <t>ubicacionEstanteria</t>
   </si>
   <si>
-    <t>(Ej: Madrid)</t>
-  </si>
-  <si>
-    <t>(Ej: 1ra)</t>
-  </si>
-  <si>
-    <t>(Ej: ...)</t>
-  </si>
-  <si>
-    <t>(Ej: 496)</t>
-  </si>
-  <si>
-    <t>(Ej: Español)</t>
-  </si>
-  <si>
-    <t>(Ej: historia,...)</t>
-  </si>
-  <si>
-    <t>(Ej: Ensayo)</t>
-  </si>
-  <si>
-    <t>(Ej: 909)</t>
-  </si>
-  <si>
-    <t>(Ej: Pasillo 1)</t>
-  </si>
-  <si>
     <t>Cien años de soledad</t>
   </si>
   <si>
@@ -254,6 +227,9 @@
   </si>
   <si>
     <t>Alba</t>
+  </si>
+  <si>
+    <t>Madrid</t>
   </si>
 </sst>
 </file>
@@ -518,15 +494,20 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,18 +554,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
@@ -593,51 +574,38 @@
         <v>1967</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>8</v>
       </c>
       <c r="F3">
         <v>1937</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -645,13 +613,13 @@
         <v>1984</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -659,19 +627,22 @@
       <c r="F4">
         <v>1949</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -679,19 +650,22 @@
       <c r="F5">
         <v>1932</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>7</v>
@@ -699,19 +673,22 @@
       <c r="F6">
         <v>1813</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -719,19 +696,22 @@
       <c r="F7">
         <v>1981</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -739,19 +719,22 @@
       <c r="F8">
         <v>1954</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -759,19 +742,22 @@
       <c r="F9">
         <v>1605</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -779,19 +765,22 @@
       <c r="F10">
         <v>-800</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <v>12</v>
@@ -799,19 +788,22 @@
       <c r="F11">
         <v>1943</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E12">
         <v>15</v>
@@ -819,19 +811,22 @@
       <c r="F12">
         <v>1997</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -839,19 +834,22 @@
       <c r="F13">
         <v>1988</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>11</v>
@@ -859,19 +857,22 @@
       <c r="F14">
         <v>1947</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -879,19 +880,22 @@
       <c r="F15">
         <v>1988</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -899,19 +903,22 @@
       <c r="F16">
         <v>1963</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -919,19 +926,22 @@
       <c r="F17">
         <v>1948</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <v>8</v>
@@ -939,19 +949,22 @@
       <c r="F18">
         <v>1982</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -959,19 +972,22 @@
       <c r="F19">
         <v>1924</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -979,25 +995,31 @@
       <c r="F20">
         <v>1953</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E21">
         <v>3</v>
       </c>
       <c r="F21">
         <v>1851</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>